<commit_message>
full testcase 3 sheet
</commit_message>
<xml_diff>
--- a/data/Login.xlsx
+++ b/data/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\eclipse_WS\Test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{4B67670A-B56B-4E4E-B7AB-E30EF14AC04E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{771522B5-C53F-41FF-950D-7306999A782B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="15720" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Testcase</t>
   </si>
@@ -46,25 +46,31 @@
     <t>Error</t>
   </si>
   <si>
-    <t xml:space="preserve">login </t>
-  </si>
-  <si>
-    <t>trungdv</t>
-  </si>
-  <si>
-    <t>trungdv123</t>
-  </si>
-  <si>
-    <t>password that you've entered is incorrect. Forgotten password?</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>The password that you've entered is incorrect. Forgotten password?</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t xml:space="preserve">login_2_3 </t>
+  </si>
+  <si>
+    <t>login_2_3</t>
+  </si>
+  <si>
+    <t>phuonglethi1901@gmail.com</t>
+  </si>
+  <si>
+    <t>E-Mail hoặc mật khẩu bị sai. Vui lòng nhập lại</t>
+  </si>
+  <si>
+    <t>Lethiphuong1901</t>
+  </si>
+  <si>
+    <t>login_4_5_6_7_8</t>
+  </si>
+  <si>
+    <t>phuonglethi@gmail.com</t>
+  </si>
+  <si>
+    <t>Lethiphuong</t>
   </si>
   <si>
     <t>Pass</t>
@@ -75,13 +81,69 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -140,12 +202,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <bgColor indexed="2"/>
+        <bgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="gray125">
-        <bgColor indexed="2"/>
+        <bgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -159,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -258,11 +320,30 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -270,15 +351,25 @@
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="true" applyFill="true" borderId="9" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="9" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,17 +648,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="62.140625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="10.140625" collapsed="true"/>
@@ -575,7 +666,7 @@
   <sheetData>
     <row ht="15.75" r="1" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -601,22 +692,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row ht="15.75" r="3" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
@@ -624,20 +713,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>10</v>
+      <c r="E3" s="1"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row ht="15.75" r="4" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
@@ -645,23 +736,116 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row ht="15.75" r="5" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row ht="15.75" r="6" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row ht="15.75" r="7" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row ht="15.75" r="8" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C3" xr:uid="{00F0E1F4-34D2-49CD-B44C-E7E53BD10673}"/>
+    <hyperlink r:id="rId2" ref="C5" xr:uid="{375DAAD9-7981-4CDB-90DB-6F28D9D09D81}"/>
+    <hyperlink r:id="rId3" ref="C6" xr:uid="{9FE741AF-2A81-4EE8-A206-A7A1B65B3284}"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>

</xml_diff>